<commit_message>
Read Master Data from XL and created mySQL tables
</commit_message>
<xml_diff>
--- a/source_data/Master Data Table for TDA2014_30_jan_2015.xlsx
+++ b/source_data/Master Data Table for TDA2014_30_jan_2015.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="28005" windowHeight="13620"/>
+    <workbookView xWindow="13200" yWindow="1320" windowWidth="28000" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="usdol 2013" sheetId="3" r:id="rId1"/>
@@ -830,9 +830,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0"/>
   </numFmts>
@@ -998,20 +998,20 @@
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1286,6 +1286,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1304,9 +1325,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1315,24 +1333,6 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1691,129 +1691,129 @@
   <dimension ref="A1:S167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="45.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="11" style="8" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="14" style="8" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.5" style="10" customWidth="1"/>
     <col min="11" max="11" width="13" style="10" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="5" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" style="6" customWidth="1"/>
-    <col min="16" max="16" width="10.28515625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="12" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="11" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="80" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="14.5" style="6" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" style="12" customWidth="1"/>
+    <col min="18" max="18" width="32.1640625" style="11" customWidth="1"/>
+    <col min="19" max="19" width="16.6640625" style="80" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37"/>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
       <c r="K1" s="15"/>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="89" t="s">
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
       <c r="R1" s="79" t="s">
         <v>222</v>
       </c>
       <c r="S1" s="79"/>
     </row>
-    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
+      <c r="A2" s="93"/>
       <c r="B2" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="C2" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="98" t="s">
+      <c r="D2" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="96" t="s">
+      <c r="E2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F2" s="88" t="s">
         <v>224</v>
       </c>
-      <c r="G2" s="92" t="s">
+      <c r="G2" s="89" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="I2" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="92" t="s">
+      <c r="J2" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="K2" s="89" t="s">
         <v>194</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="100" t="s">
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="94" t="s">
+      <c r="P2" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="95" t="s">
+      <c r="Q2" s="101" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="101" t="s">
+      <c r="R2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="97" t="s">
+      <c r="S2" s="86" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
+    <row r="3" spans="1:19" ht="29.25" customHeight="1">
+      <c r="A3" s="93"/>
       <c r="B3" s="37"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
       <c r="L3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1823,13 +1823,13 @@
       <c r="N3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="100"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="97"/>
-    </row>
-    <row r="4" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="91"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="86"/>
+    </row>
+    <row r="4" spans="1:19" s="6" customFormat="1">
       <c r="A4" s="44" t="s">
         <v>14</v>
       </c>
@@ -1878,7 +1878,7 @@
       <c r="R4" s="85"/>
       <c r="S4" s="13"/>
     </row>
-    <row r="5" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="13" customFormat="1">
       <c r="A5" s="21" t="s">
         <v>15</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="R5" s="75"/>
       <c r="S5" s="81"/>
     </row>
-    <row r="6" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="6" customFormat="1">
       <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>100.2</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="6" customFormat="1">
       <c r="A7" s="21" t="s">
         <v>19</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="6" customFormat="1">
       <c r="A8" s="21" t="s">
         <v>20</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>78.7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="6" customFormat="1">
       <c r="A9" s="44" t="s">
         <v>21</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>109.3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="6" customFormat="1">
       <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="6" customFormat="1">
       <c r="A11" s="21" t="s">
         <v>23</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="6" customFormat="1">
       <c r="A12" s="21" t="s">
         <v>25</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="R12" s="76"/>
       <c r="S12" s="81"/>
     </row>
-    <row r="13" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="7" customFormat="1">
       <c r="A13" s="23" t="s">
         <v>26</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>74.599999999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="6" customFormat="1">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="6" customFormat="1">
       <c r="A15" s="44" t="s">
         <v>30</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>103.3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="40" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>32</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>116.1</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" s="6" customFormat="1">
       <c r="A17" s="44" t="s">
         <v>34</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" s="6" customFormat="1">
       <c r="A18" s="21" t="s">
         <v>36</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>101.3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" s="6" customFormat="1">
       <c r="A19" s="21" t="s">
         <v>38</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>92.3</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" s="6" customFormat="1">
       <c r="A20" s="21" t="s">
         <v>40</v>
       </c>
@@ -2648,7 +2648,7 @@
       <c r="R20" s="76"/>
       <c r="S20" s="81"/>
     </row>
-    <row r="21" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" s="6" customFormat="1">
       <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>94.7</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" s="13" customFormat="1">
       <c r="A22" s="21" t="s">
         <v>42</v>
       </c>
@@ -2730,7 +2730,7 @@
       <c r="R22" s="76"/>
       <c r="S22" s="81"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="29" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="Q23" s="32"/>
       <c r="R23" s="76"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="29" t="s">
         <v>45</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>92.9</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" s="40" customFormat="1">
       <c r="A25" s="21" t="s">
         <v>46</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>57.6</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" s="6" customFormat="1">
       <c r="A26" s="21" t="s">
         <v>47</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" s="6" customFormat="1">
       <c r="A27" s="44" t="s">
         <v>48</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>98.1</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" s="40" customFormat="1">
       <c r="A28" s="21" t="s">
         <v>51</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" s="6" customFormat="1">
       <c r="A29" s="21" t="s">
         <v>52</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" s="6" customFormat="1">
       <c r="A30" s="44" t="s">
         <v>54</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" s="6" customFormat="1">
       <c r="A31" s="44" t="s">
         <v>55</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" s="6" customFormat="1">
       <c r="A32" s="44" t="s">
         <v>56</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>97.3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="6" customFormat="1">
       <c r="A33" s="21" t="s">
         <v>57</v>
       </c>
@@ -3260,7 +3260,7 @@
       <c r="R33" s="76"/>
       <c r="S33" s="81"/>
     </row>
-    <row r="34" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" s="6" customFormat="1">
       <c r="A34" s="21" t="s">
         <v>58</v>
       </c>
@@ -3283,7 +3283,7 @@
       <c r="R34" s="76"/>
       <c r="S34" s="81"/>
     </row>
-    <row r="35" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" s="40" customFormat="1">
       <c r="A35" s="23" t="s">
         <v>59</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" s="6" customFormat="1">
       <c r="A36" s="44" t="s">
         <v>60</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="37" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" s="6" customFormat="1">
       <c r="A37" s="44" t="s">
         <v>61</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" s="6" customFormat="1">
       <c r="A38" s="21" t="s">
         <v>62</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>72.8</v>
       </c>
     </row>
-    <row r="39" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" s="6" customFormat="1">
       <c r="A39" s="21" t="s">
         <v>63</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>102.7</v>
       </c>
     </row>
-    <row r="40" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" s="6" customFormat="1">
       <c r="A40" s="44" t="s">
         <v>64</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>95.2</v>
       </c>
     </row>
-    <row r="41" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" s="6" customFormat="1">
       <c r="A41" s="44" t="s">
         <v>65</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="42" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" s="6" customFormat="1">
       <c r="A42" s="21" t="s">
         <v>66</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>93.2</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" s="6" customFormat="1">
       <c r="A43" s="21" t="s">
         <v>67</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" s="6" customFormat="1">
       <c r="A44" s="21" t="s">
         <v>68</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" s="40" customFormat="1">
       <c r="A45" s="21" t="s">
         <v>215</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>90.3</v>
       </c>
     </row>
-    <row r="46" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" s="6" customFormat="1">
       <c r="A46" s="21" t="s">
         <v>69</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" s="40" customFormat="1">
       <c r="A47" s="43" t="s">
         <v>71</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>110.9</v>
       </c>
     </row>
-    <row r="48" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" s="6" customFormat="1">
       <c r="A48" s="21" t="s">
         <v>73</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="49" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" s="13" customFormat="1">
       <c r="A49" s="21" t="s">
         <v>74</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" s="29" t="s">
         <v>76</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>54.8</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="29" t="s">
         <v>77</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19">
       <c r="A52" s="29" t="s">
         <v>191</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19">
       <c r="A53" s="29" t="s">
         <v>78</v>
       </c>
@@ -4167,7 +4167,7 @@
       <c r="Q53" s="32"/>
       <c r="R53" s="76"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" s="29" t="s">
         <v>79</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>103.6</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19">
       <c r="A55" s="53" t="s">
         <v>80</v>
       </c>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="R55" s="76"/>
     </row>
-    <row r="56" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" s="6" customFormat="1">
       <c r="A56" s="21" t="s">
         <v>81</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="57" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" s="6" customFormat="1">
       <c r="A57" s="21" t="s">
         <v>83</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>108.1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" s="6" customFormat="1">
       <c r="A58" s="21" t="s">
         <v>84</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="59" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" s="6" customFormat="1">
       <c r="A59" s="21" t="s">
         <v>85</v>
       </c>
@@ -4423,7 +4423,7 @@
       <c r="Q59" s="18"/>
       <c r="S59" s="81"/>
     </row>
-    <row r="60" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" s="6" customFormat="1">
       <c r="A60" s="21" t="s">
         <v>86</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>111.5</v>
       </c>
     </row>
-    <row r="61" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" s="6" customFormat="1">
       <c r="A61" s="44" t="s">
         <v>87</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="62" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" s="40" customFormat="1">
       <c r="A62" s="44" t="s">
         <v>88</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" s="6" customFormat="1">
       <c r="A63" s="21" t="s">
         <v>89</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" s="6" customFormat="1">
       <c r="A64" s="21" t="s">
         <v>90</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>85.3</v>
       </c>
     </row>
-    <row r="65" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" s="6" customFormat="1">
       <c r="A65" s="44" t="s">
         <v>92</v>
       </c>
@@ -4717,7 +4717,7 @@
       <c r="R65" s="76"/>
       <c r="S65" s="81"/>
     </row>
-    <row r="66" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" s="6" customFormat="1">
       <c r="A66" s="21" t="s">
         <v>93</v>
       </c>
@@ -4740,7 +4740,7 @@
       <c r="R66" s="76"/>
       <c r="S66" s="81"/>
     </row>
-    <row r="67" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" s="6" customFormat="1">
       <c r="A67" s="44" t="s">
         <v>94</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="68" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" s="6" customFormat="1">
       <c r="A68" s="44" t="s">
         <v>95</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>96.5</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" s="6" customFormat="1">
       <c r="A69" s="21" t="s">
         <v>96</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="70" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" s="40" customFormat="1">
       <c r="A70" s="21" t="s">
         <v>97</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>66.3</v>
       </c>
     </row>
-    <row r="71" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" s="6" customFormat="1">
       <c r="A71" s="44" t="s">
         <v>98</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" s="6" customFormat="1">
       <c r="A72" s="21" t="s">
         <v>99</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>92.8</v>
       </c>
     </row>
-    <row r="73" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" s="6" customFormat="1">
       <c r="A73" s="21" t="s">
         <v>100</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>102.2</v>
       </c>
     </row>
-    <row r="74" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" s="6" customFormat="1">
       <c r="A74" s="21" t="s">
         <v>101</v>
       </c>
@@ -5194,7 +5194,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="75" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" s="6" customFormat="1">
       <c r="A75" s="21" t="s">
         <v>102</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>115.2</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" s="6" customFormat="1">
       <c r="A76" s="21" t="s">
         <v>103</v>
       </c>
@@ -5244,7 +5244,7 @@
       <c r="R76" s="76"/>
       <c r="S76" s="81"/>
     </row>
-    <row r="77" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" s="6" customFormat="1">
       <c r="A77" s="21" t="s">
         <v>104</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>97.7</v>
       </c>
     </row>
-    <row r="78" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" s="40" customFormat="1">
       <c r="A78" s="21" t="s">
         <v>218</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="79" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" s="6" customFormat="1">
       <c r="A79" s="21" t="s">
         <v>105</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>86.2</v>
       </c>
     </row>
-    <row r="80" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" s="6" customFormat="1">
       <c r="A80" s="21" t="s">
         <v>106</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="81" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" s="6" customFormat="1">
       <c r="A81" s="21" t="s">
         <v>108</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>65.2</v>
       </c>
     </row>
-    <row r="82" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" s="6" customFormat="1">
       <c r="A82" s="44" t="s">
         <v>109</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>74.5</v>
       </c>
     </row>
-    <row r="83" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" s="6" customFormat="1">
       <c r="A83" s="21" t="s">
         <v>110</v>
       </c>
@@ -5607,7 +5607,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="84" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" s="40" customFormat="1">
       <c r="A84" s="21" t="s">
         <v>111</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>74.2</v>
       </c>
     </row>
-    <row r="85" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" s="6" customFormat="1">
       <c r="A85" s="21" t="s">
         <v>112</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>109.9</v>
       </c>
     </row>
-    <row r="86" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" s="6" customFormat="1">
       <c r="A86" s="44" t="s">
         <v>113</v>
       </c>
@@ -5776,7 +5776,7 @@
         <v>58.7</v>
       </c>
     </row>
-    <row r="87" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" s="6" customFormat="1">
       <c r="A87" s="21" t="s">
         <v>114</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>99.3</v>
       </c>
     </row>
-    <row r="88" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" s="6" customFormat="1">
       <c r="A88" s="21" t="s">
         <v>115</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="89" spans="1:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" s="13" customFormat="1">
       <c r="A89" s="21" t="s">
         <v>116</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>99.1</v>
       </c>
     </row>
-    <row r="90" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" s="6" customFormat="1">
       <c r="A90" s="21" t="s">
         <v>187</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>89.6</v>
       </c>
     </row>
-    <row r="91" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" s="40" customFormat="1">
       <c r="A91" s="21" t="s">
         <v>117</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>130.19999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" s="6" customFormat="1">
       <c r="A92" s="21" t="s">
         <v>118</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="93" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" s="6" customFormat="1">
       <c r="A93" s="21" t="s">
         <v>119</v>
       </c>
@@ -6113,7 +6113,7 @@
         <v>68.900000000000006</v>
       </c>
     </row>
-    <row r="94" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" s="6" customFormat="1">
       <c r="A94" s="21" t="s">
         <v>120</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>98.9</v>
       </c>
     </row>
-    <row r="95" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" s="6" customFormat="1">
       <c r="A95" s="21" t="s">
         <v>121</v>
       </c>
@@ -6219,7 +6219,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="96" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" s="6" customFormat="1">
       <c r="A96" s="21" t="s">
         <v>122</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="97" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" s="40" customFormat="1">
       <c r="A97" s="21" t="s">
         <v>123</v>
       </c>
@@ -6305,7 +6305,7 @@
         <v>99.8</v>
       </c>
     </row>
-    <row r="98" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" s="6" customFormat="1">
       <c r="A98" s="44" t="s">
         <v>124</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="99" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" s="6" customFormat="1">
       <c r="A99" s="44" t="s">
         <v>125</v>
       </c>
@@ -6417,7 +6417,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="100" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" s="40" customFormat="1">
       <c r="A100" s="21" t="s">
         <v>126</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" s="6" customFormat="1">
       <c r="A101" s="21" t="s">
         <v>127</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>115.4</v>
       </c>
     </row>
-    <row r="102" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" s="6" customFormat="1">
       <c r="A102" s="21" t="s">
         <v>128</v>
       </c>
@@ -6526,7 +6526,7 @@
       <c r="R102" s="76"/>
       <c r="S102" s="81"/>
     </row>
-    <row r="103" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" s="6" customFormat="1">
       <c r="A103" s="21" t="s">
         <v>129</v>
       </c>
@@ -6553,7 +6553,7 @@
         <v>103.7</v>
       </c>
     </row>
-    <row r="104" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" s="6" customFormat="1">
       <c r="A104" s="21" t="s">
         <v>130</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>71.900000000000006</v>
       </c>
     </row>
-    <row r="105" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" s="40" customFormat="1">
       <c r="A105" s="44" t="s">
         <v>131</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>97.7</v>
       </c>
     </row>
-    <row r="106" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" s="6" customFormat="1">
       <c r="A106" s="21" t="s">
         <v>132</v>
       </c>
@@ -6698,7 +6698,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="107" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" s="6" customFormat="1">
       <c r="A107" s="21" t="s">
         <v>133</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="108" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" s="40" customFormat="1">
       <c r="A108" s="21" t="s">
         <v>134</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="109" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" s="6" customFormat="1">
       <c r="A109" s="44" t="s">
         <v>135</v>
       </c>
@@ -6875,7 +6875,7 @@
         <v>91.3</v>
       </c>
     </row>
-    <row r="110" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" s="6" customFormat="1">
       <c r="A110" s="21" t="s">
         <v>136</v>
       </c>
@@ -6898,7 +6898,7 @@
       <c r="R110" s="76"/>
       <c r="S110" s="81"/>
     </row>
-    <row r="111" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" s="6" customFormat="1">
       <c r="A111" s="21" t="s">
         <v>137</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>97.1</v>
       </c>
     </row>
-    <row r="112" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" s="40" customFormat="1">
       <c r="A112" s="21" t="s">
         <v>138</v>
       </c>
@@ -6984,7 +6984,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="113" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" s="6" customFormat="1">
       <c r="A113" s="21" t="s">
         <v>139</v>
       </c>
@@ -7007,7 +7007,7 @@
       <c r="R113" s="76"/>
       <c r="S113" s="81"/>
     </row>
-    <row r="114" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" s="6" customFormat="1">
       <c r="A114" s="21" t="s">
         <v>140</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>102.4</v>
       </c>
     </row>
-    <row r="115" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" s="6" customFormat="1">
       <c r="A115" s="21" t="s">
         <v>141</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" s="6" customFormat="1">
       <c r="A116" s="44" t="s">
         <v>142</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>60.5</v>
       </c>
     </row>
-    <row r="117" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" s="6" customFormat="1">
       <c r="A117" s="21" t="s">
         <v>143</v>
       </c>
@@ -7199,7 +7199,7 @@
         <v>93.2</v>
       </c>
     </row>
-    <row r="118" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="15.75" customHeight="1">
       <c r="A118" s="29" t="s">
         <v>144</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>104.5</v>
       </c>
     </row>
-    <row r="119" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" s="40" customFormat="1">
       <c r="A119" s="57" t="s">
         <v>145</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19">
       <c r="A120" s="29" t="s">
         <v>146</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="121" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" s="6" customFormat="1">
       <c r="A121" s="21" t="s">
         <v>147</v>
       </c>
@@ -7361,7 +7361,7 @@
       <c r="R121" s="77"/>
       <c r="S121" s="81"/>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19">
       <c r="A122" s="29" t="s">
         <v>148</v>
       </c>
@@ -7388,7 +7388,7 @@
         <v>98.5</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19">
       <c r="A123" s="29" t="s">
         <v>149</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>96.8</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19">
       <c r="A124" s="29" t="s">
         <v>150</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>92.6</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19">
       <c r="A125" s="53" t="s">
         <v>151</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19">
       <c r="A126" s="29" t="s">
         <v>152</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>98.9</v>
       </c>
     </row>
-    <row r="127" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" s="6" customFormat="1">
       <c r="A127" s="21" t="s">
         <v>153</v>
       </c>
@@ -7609,7 +7609,7 @@
       <c r="R127" s="77"/>
       <c r="S127" s="81"/>
     </row>
-    <row r="128" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" s="6" customFormat="1">
       <c r="A128" s="21" t="s">
         <v>155</v>
       </c>
@@ -7668,7 +7668,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="129" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" s="40" customFormat="1">
       <c r="A129" s="21" t="s">
         <v>156</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="130" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" s="6" customFormat="1">
       <c r="A130" s="21" t="s">
         <v>157</v>
       </c>
@@ -7784,7 +7784,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="131" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" s="6" customFormat="1">
       <c r="A131" s="21" t="s">
         <v>158</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>106.7</v>
       </c>
     </row>
-    <row r="132" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" s="6" customFormat="1">
       <c r="A132" s="21" t="s">
         <v>159</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>97.6</v>
       </c>
     </row>
-    <row r="133" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" s="40" customFormat="1">
       <c r="A133" s="23" t="s">
         <v>160</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="134" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" s="6" customFormat="1">
       <c r="A134" s="23" t="s">
         <v>161</v>
       </c>
@@ -7998,7 +7998,7 @@
       <c r="R134" s="77"/>
       <c r="S134" s="81"/>
     </row>
-    <row r="135" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" s="40" customFormat="1">
       <c r="A135" s="43" t="s">
         <v>162</v>
       </c>
@@ -8057,7 +8057,7 @@
         <v>77.400000000000006</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19">
       <c r="A136" s="29" t="s">
         <v>163</v>
       </c>
@@ -8079,7 +8079,7 @@
       <c r="Q136" s="68"/>
       <c r="R136" s="77"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19">
       <c r="A137" s="29" t="s">
         <v>164</v>
       </c>
@@ -8106,7 +8106,7 @@
         <v>98.6</v>
       </c>
     </row>
-    <row r="138" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" s="6" customFormat="1">
       <c r="A138" s="21" t="s">
         <v>165</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>94.8</v>
       </c>
     </row>
-    <row r="139" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" s="6" customFormat="1">
       <c r="A139" s="44" t="s">
         <v>166</v>
       </c>
@@ -8212,7 +8212,7 @@
         <v>101.7</v>
       </c>
     </row>
-    <row r="140" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" s="6" customFormat="1">
       <c r="A140" s="21" t="s">
         <v>167</v>
       </c>
@@ -8271,7 +8271,7 @@
         <v>101.4</v>
       </c>
     </row>
-    <row r="141" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" s="6" customFormat="1">
       <c r="A141" s="21" t="s">
         <v>168</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>91.7</v>
       </c>
     </row>
-    <row r="142" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" s="6" customFormat="1">
       <c r="A142" s="21" t="s">
         <v>169</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>99.2</v>
       </c>
     </row>
-    <row r="143" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" s="40" customFormat="1">
       <c r="A143" s="21" t="s">
         <v>170</v>
       </c>
@@ -8384,7 +8384,7 @@
         <v>53.1</v>
       </c>
     </row>
-    <row r="144" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" s="6" customFormat="1">
       <c r="A144" s="44" t="s">
         <v>171</v>
       </c>
@@ -8437,7 +8437,7 @@
         <v>102.8</v>
       </c>
     </row>
-    <row r="145" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" s="6" customFormat="1">
       <c r="A145" s="21" t="s">
         <v>172</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>104.3</v>
       </c>
     </row>
-    <row r="146" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" s="6" customFormat="1">
       <c r="A146" s="21" t="s">
         <v>173</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>91.8</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19">
       <c r="A147" s="29" t="s">
         <v>174</v>
       </c>
@@ -8576,7 +8576,7 @@
         <v>83.6</v>
       </c>
     </row>
-    <row r="148" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" s="6" customFormat="1">
       <c r="A148" s="21" t="s">
         <v>175</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="149" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" s="6" customFormat="1">
       <c r="A149" s="44" t="s">
         <v>188</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>101.2</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19">
       <c r="A150" s="29" t="s">
         <v>176</v>
       </c>
@@ -8716,7 +8716,7 @@
       <c r="Q150" s="32"/>
       <c r="R150" s="76"/>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19">
       <c r="A151" s="29" t="s">
         <v>177</v>
       </c>
@@ -8738,7 +8738,7 @@
       <c r="Q151" s="32"/>
       <c r="R151" s="76"/>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19">
       <c r="A152" s="29" t="s">
         <v>178</v>
       </c>
@@ -8760,7 +8760,7 @@
       <c r="Q152" s="32"/>
       <c r="R152" s="76"/>
     </row>
-    <row r="153" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" s="40" customFormat="1">
       <c r="A153" s="21" t="s">
         <v>179</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="154" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" s="6" customFormat="1">
       <c r="A154" s="21" t="s">
         <v>180</v>
       </c>
@@ -8878,7 +8878,7 @@
         <v>91.3</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19">
       <c r="A155" s="29" t="s">
         <v>181</v>
       </c>
@@ -8900,40 +8900,40 @@
       <c r="Q155" s="32"/>
       <c r="R155" s="76"/>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19">
       <c r="R156" s="78"/>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19">
       <c r="R157" s="78"/>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19">
       <c r="R158" s="78"/>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19">
       <c r="R159" s="78"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19">
       <c r="R160" s="78"/>
     </row>
-    <row r="161" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="161" spans="18:18">
       <c r="R161" s="78"/>
     </row>
-    <row r="162" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="162" spans="18:18">
       <c r="R162" s="78"/>
     </row>
-    <row r="163" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="163" spans="18:18">
       <c r="R163" s="78"/>
     </row>
-    <row r="164" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="164" spans="18:18">
       <c r="R164" s="78"/>
     </row>
-    <row r="165" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="165" spans="18:18">
       <c r="R165" s="78"/>
     </row>
-    <row r="166" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="166" spans="18:18">
       <c r="R166" s="78"/>
     </row>
-    <row r="167" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="167" spans="18:18">
       <c r="R167" s="78"/>
     </row>
   </sheetData>
@@ -8951,15 +8951,6 @@
     <filterColumn colId="15" showButton="0"/>
   </autoFilter>
   <mergeCells count="19">
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="L1:N1"/>
@@ -8970,6 +8961,15 @@
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="52" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>

</xml_diff>